<commit_message>
batch 8 scenarios completed
</commit_message>
<xml_diff>
--- a/src/test/resources/LMSData.xlsx
+++ b/src/test/resources/LMSData.xlsx
@@ -4,7 +4,7 @@
   <workbookPr/>
   <sheets>
     <sheet state="visible" name="Login" sheetId="1" r:id="rId4"/>
-    <sheet state="visible" name="Program" sheetId="2" r:id="rId5"/>
+    <sheet state="visible" name="Program_sheet" sheetId="2" r:id="rId5"/>
     <sheet state="visible" name="Batch" sheetId="3" r:id="rId6"/>
     <sheet state="visible" name="Class" sheetId="4" r:id="rId7"/>
   </sheets>
@@ -14,23 +14,95 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="48">
   <si>
     <t>Program Name</t>
   </si>
   <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>LMSProgram</t>
+  </si>
+  <si>
+    <t>LMS</t>
+  </si>
+  <si>
+    <t>Active</t>
+  </si>
+  <si>
+    <t>valid</t>
+  </si>
+  <si>
+    <t>save</t>
+  </si>
+  <si>
+    <t>L8</t>
+  </si>
+  <si>
+    <t>Learning</t>
+  </si>
+  <si>
+    <t>Inactive</t>
+  </si>
+  <si>
+    <t>Management</t>
+  </si>
+  <si>
+    <t>cancel</t>
+  </si>
+  <si>
+    <t>L9</t>
+  </si>
+  <si>
+    <t>systems</t>
+  </si>
+  <si>
+    <t>cross</t>
+  </si>
+  <si>
+    <t>L</t>
+  </si>
+  <si>
+    <t>Training</t>
+  </si>
+  <si>
+    <t>Invalid- invalid char in name</t>
+  </si>
+  <si>
+    <t>ChatBot</t>
+  </si>
+  <si>
+    <t>testing</t>
+  </si>
+  <si>
+    <t>Invalid- blank Status field</t>
+  </si>
+  <si>
+    <t>automation</t>
+  </si>
+  <si>
+    <t>Invalid- blank Name field</t>
+  </si>
+  <si>
+    <t>PlayWright</t>
+  </si>
+  <si>
+    <t>Invalid-blank Description field</t>
+  </si>
+  <si>
     <t>Batch Name</t>
   </si>
   <si>
-    <t>Description</t>
-  </si>
-  <si>
-    <t>Status</t>
-  </si>
-  <si>
     <t>Number of Classes</t>
   </si>
   <si>
+    <t>Valid</t>
+  </si>
+  <si>
     <t>AzureP</t>
   </si>
   <si>
@@ -40,14 +112,59 @@
     <t>ACTIVE</t>
   </si>
   <si>
-    <t>Azure Batch new</t>
+    <t>Invalid</t>
+  </si>
+  <si>
+    <t>abc</t>
+  </si>
+  <si>
+    <t>Mandatory</t>
+  </si>
+  <si>
+    <t>SeleniumP</t>
+  </si>
+  <si>
+    <t>Selenium Automation</t>
+  </si>
+  <si>
+    <t>All</t>
+  </si>
+  <si>
+    <t>BDD Automation</t>
+  </si>
+  <si>
+    <t>Blank ProgramName</t>
+  </si>
+  <si>
+    <t>BDD</t>
+  </si>
+  <si>
+    <t>Blank Batch Name</t>
+  </si>
+  <si>
+    <t>Blank Description</t>
+  </si>
+  <si>
+    <t>Blank Status</t>
+  </si>
+  <si>
+    <t>Blank Number of Classes</t>
+  </si>
+  <si>
+    <t>Edit Mandatory</t>
+  </si>
+  <si>
+    <t>PlayWrightAuto</t>
+  </si>
+  <si>
+    <t>search</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="2">
+  <fonts count="7">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -55,8 +172,33 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <color theme="1"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <b/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <color theme="1"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -73,21 +215,43 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="13">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="right" readingOrder="0" vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="right" vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" vertical="bottom"/>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="right" readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -330,7 +494,173 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
-  <sheetData/>
+  <cols>
+    <col customWidth="1" min="1" max="1" width="15.63"/>
+    <col customWidth="1" min="2" max="2" width="14.63"/>
+    <col customWidth="1" min="3" max="3" width="16.0"/>
+    <col customWidth="1" min="4" max="4" width="24.5"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
+      <c r="J1" s="4"/>
+      <c r="K1" s="4"/>
+      <c r="L1" s="4"/>
+      <c r="M1" s="4"/>
+      <c r="N1" s="4"/>
+      <c r="O1" s="4"/>
+      <c r="P1" s="4"/>
+      <c r="Q1" s="4"/>
+      <c r="R1" s="4"/>
+      <c r="S1" s="4"/>
+      <c r="T1" s="4"/>
+      <c r="U1" s="4"/>
+      <c r="V1" s="4"/>
+      <c r="W1" s="4"/>
+    </row>
+    <row r="2">
+      <c r="A2" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="B8" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
@@ -344,56 +674,233 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <cols>
+    <col customWidth="1" min="1" max="1" width="22.75"/>
+    <col customWidth="1" min="4" max="4" width="14.88"/>
+    <col customWidth="1" min="6" max="6" width="16.63"/>
+  </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2"/>
+      <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
+      <c r="F1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
+      <c r="J1" s="4"/>
+      <c r="K1" s="4"/>
+      <c r="L1" s="4"/>
+      <c r="M1" s="4"/>
+      <c r="N1" s="4"/>
+      <c r="O1" s="4"/>
+      <c r="P1" s="4"/>
+      <c r="Q1" s="4"/>
+      <c r="R1" s="4"/>
+      <c r="S1" s="4"/>
+      <c r="T1" s="4"/>
+      <c r="U1" s="4"/>
+      <c r="V1" s="4"/>
+      <c r="W1" s="4"/>
+      <c r="X1" s="4"/>
+      <c r="Y1" s="4"/>
+      <c r="Z1" s="4"/>
+      <c r="AA1" s="4"/>
     </row>
     <row r="2">
-      <c r="A2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" s="2">
-        <v>400.0</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2" s="3">
+      <c r="A2" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2" s="9">
+        <v>800.0</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="F2" s="10">
         <v>2.0</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" s="2">
-        <v>201.0</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E3" s="2">
-        <v>3.0</v>
+      <c r="A3" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="D3" s="7">
+        <v>23244.0</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="F3" s="11" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C4" s="12">
+        <v>297.0</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="F4" s="5">
+        <v>5.0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C5" s="12">
+        <v>298.0</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="F5" s="5">
+        <v>5.0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C6" s="5">
+        <v>30.0</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="F6" s="5">
+        <v>5.0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="F7" s="5">
+        <v>5.0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C8" s="5">
+        <v>30.0</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="F8" s="5">
+        <v>5.0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C9" s="5">
+        <v>30.0</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="F9" s="5">
+        <v>5.0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C10" s="5">
+        <v>30.0</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="F11" s="5">
+        <v>28.0</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added log line and removed unwanted lines for batch module
</commit_message>
<xml_diff>
--- a/src/test/resources/LMSData.xlsx
+++ b/src/test/resources/LMSData.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="58">
   <si>
     <t>name</t>
   </si>
@@ -85,10 +85,10 @@
     <t>Program Status</t>
   </si>
   <si>
-    <t>LMSProgram</t>
-  </si>
-  <si>
-    <t>LMS</t>
+    <t>LMSPrograms</t>
+  </si>
+  <si>
+    <t>LMSTeach</t>
   </si>
   <si>
     <t>Active</t>
@@ -122,9 +122,6 @@
   </si>
   <si>
     <t>automation</t>
-  </si>
-  <si>
-    <t>PlayWright</t>
   </si>
   <si>
     <t>Tableau</t>
@@ -165,7 +162,7 @@
     <t>Valid</t>
   </si>
   <si>
-    <t>InformationTechPath</t>
+    <t>MobileSeleniumAuto</t>
   </si>
   <si>
     <t>Azure Batch</t>
@@ -219,7 +216,7 @@
     <t>search</t>
   </si>
   <si>
-    <t>ITPath</t>
+    <t>selenium</t>
   </si>
 </sst>
 </file>
@@ -291,7 +288,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="20">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -330,6 +327,9 @@
       <alignment readingOrder="0" vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="right" readingOrder="0" vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -344,6 +344,7 @@
     <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -743,20 +744,12 @@
         <v>24</v>
       </c>
     </row>
-    <row r="8">
-      <c r="A8" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
     <row r="9">
       <c r="A9" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>30</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>31</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>18</v>
@@ -775,10 +768,10 @@
     </row>
     <row r="11">
       <c r="A11" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>32</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>33</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>24</v>
@@ -786,7 +779,7 @@
     </row>
     <row r="14">
       <c r="D14" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -815,16 +808,16 @@
         <v>13</v>
       </c>
       <c r="C1" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="D1" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="D1" s="11" t="s">
+      <c r="E1" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="F1" s="11" t="s">
         <v>37</v>
-      </c>
-      <c r="F1" s="11" t="s">
-        <v>38</v>
       </c>
       <c r="G1" s="9"/>
       <c r="H1" s="9"/>
@@ -850,59 +843,59 @@
     </row>
     <row r="2">
       <c r="A2" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="B2" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="B2" s="12" t="s">
+      <c r="C2" s="14">
+        <v>9.0</v>
+      </c>
+      <c r="D2" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="C2" s="13">
-        <v>810.0</v>
-      </c>
-      <c r="D2" s="14" t="s">
+      <c r="E2" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="E2" s="14" t="s">
-        <v>42</v>
-      </c>
-      <c r="F2" s="15">
+      <c r="F2" s="16">
         <v>2.0</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="B3" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="C3" s="17" t="s">
         <v>43</v>
-      </c>
-      <c r="B3" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="C3" s="16" t="s">
-        <v>44</v>
       </c>
       <c r="D3" s="12">
         <v>23244.0</v>
       </c>
-      <c r="E3" s="14" t="s">
-        <v>42</v>
-      </c>
-      <c r="F3" s="16" t="s">
-        <v>44</v>
+      <c r="E3" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="F3" s="17" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B4" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="C4" s="18">
+        <v>11.0</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B4" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="C4" s="17">
-        <v>319.0</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>46</v>
-      </c>
       <c r="E4" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F4" s="1">
         <v>5.0</v>
@@ -910,19 +903,19 @@
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B5" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="C5" s="18">
+        <v>12.0</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="B5" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="C5" s="17">
-        <v>320.0</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>48</v>
-      </c>
       <c r="E5" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F5" s="1">
         <v>5.0</v>
@@ -930,16 +923,17 @@
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>49</v>
-      </c>
+        <v>48</v>
+      </c>
+      <c r="B6" s="19"/>
       <c r="C6" s="1">
         <v>30.0</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F6" s="1">
         <v>5.0</v>
@@ -947,16 +941,16 @@
     </row>
     <row r="7">
       <c r="A7" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="B7" s="12" t="s">
-        <v>40</v>
+        <v>50</v>
+      </c>
+      <c r="B7" s="13" t="s">
+        <v>39</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F7" s="1">
         <v>5.0</v>
@@ -964,16 +958,16 @@
     </row>
     <row r="8">
       <c r="A8" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="B8" s="12" t="s">
-        <v>40</v>
+        <v>51</v>
+      </c>
+      <c r="B8" s="13" t="s">
+        <v>39</v>
       </c>
       <c r="C8" s="1">
         <v>30.0</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F8" s="1">
         <v>5.0</v>
@@ -981,16 +975,16 @@
     </row>
     <row r="9">
       <c r="A9" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="B9" s="12" t="s">
-        <v>40</v>
+        <v>52</v>
+      </c>
+      <c r="B9" s="13" t="s">
+        <v>39</v>
       </c>
       <c r="C9" s="1">
         <v>30.0</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F9" s="1">
         <v>5.0</v>
@@ -998,27 +992,27 @@
     </row>
     <row r="10">
       <c r="A10" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="B10" s="12" t="s">
-        <v>40</v>
+        <v>53</v>
+      </c>
+      <c r="B10" s="13" t="s">
+        <v>39</v>
       </c>
       <c r="C10" s="1">
         <v>30.0</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D11" s="1" t="s">
         <v>55</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>56</v>
       </c>
       <c r="F11" s="1">
         <v>28.0</v>
@@ -1026,10 +1020,10 @@
     </row>
     <row r="12">
       <c r="A12" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C12" s="13" t="s">
         <v>57</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>58</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
increased wait time for add new batch popup
</commit_message>
<xml_diff>
--- a/src/test/resources/LMSData.xlsx
+++ b/src/test/resources/LMSData.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="61">
   <si>
     <t>name</t>
   </si>
@@ -85,10 +85,10 @@
     <t>Program Status</t>
   </si>
   <si>
-    <t>LMSPrograms</t>
-  </si>
-  <si>
-    <t>LMSTeach</t>
+    <t>Yxyxyx</t>
+  </si>
+  <si>
+    <t>ababab</t>
   </si>
   <si>
     <t>Active</t>
@@ -124,6 +124,12 @@
     <t>automation</t>
   </si>
   <si>
+    <t>8playwright8</t>
+  </si>
+  <si>
+    <t>auto</t>
+  </si>
+  <si>
     <t>Tableau</t>
   </si>
   <si>
@@ -133,18 +139,13 @@
     <t>SMPO</t>
   </si>
   <si>
-    <t>Y</t>
-  </si>
-  <si>
-    <t>valid
-valid
-valid
-valid
-Invalid- invalid char in name
-Invalid- invalid char in name
-Invalid- blank Status field
-Invalid- blank Name field
-Invalid-blank Description field</t>
+    <t>%G</t>
+  </si>
+  <si>
+    <t>ML</t>
+  </si>
+  <si>
+    <t>Machines</t>
   </si>
   <si>
     <t>Batch Name</t>
@@ -162,7 +163,7 @@
     <t>Valid</t>
   </si>
   <si>
-    <t>MobileSeleniumAuto</t>
+    <t>activa</t>
   </si>
   <si>
     <t>Azure Batch</t>
@@ -744,12 +745,23 @@
         <v>24</v>
       </c>
     </row>
+    <row r="8">
+      <c r="A8" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
     <row r="9">
       <c r="A9" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>18</v>
@@ -768,19 +780,28 @@
     </row>
     <row r="11">
       <c r="A11" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>24</v>
       </c>
     </row>
+    <row r="12">
+      <c r="A12" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
     <row r="14">
-      <c r="D14" s="1" t="s">
-        <v>33</v>
-      </c>
+      <c r="D14" s="1"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>
@@ -808,16 +829,16 @@
         <v>13</v>
       </c>
       <c r="C1" s="11" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="D1" s="11" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="E1" s="11" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="F1" s="11" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="G1" s="9"/>
       <c r="H1" s="9"/>
@@ -843,19 +864,19 @@
     </row>
     <row r="2">
       <c r="A2" s="12" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="C2" s="14">
-        <v>9.0</v>
+        <v>13.0</v>
       </c>
       <c r="D2" s="15" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="E2" s="15" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="F2" s="16">
         <v>2.0</v>
@@ -863,39 +884,39 @@
     </row>
     <row r="3">
       <c r="A3" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="B3" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="B3" s="13" t="s">
-        <v>39</v>
-      </c>
       <c r="C3" s="17" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="D3" s="12">
         <v>23244.0</v>
       </c>
       <c r="E3" s="15" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="F3" s="17" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B4" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="C4" s="18">
+        <v>14.0</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>44</v>
-      </c>
-      <c r="B4" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="C4" s="18">
-        <v>11.0</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>41</v>
       </c>
       <c r="F4" s="1">
         <v>5.0</v>
@@ -903,19 +924,19 @@
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="C5" s="18">
-        <v>12.0</v>
+        <v>15.0</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="F5" s="1">
         <v>5.0</v>
@@ -923,17 +944,17 @@
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="B6" s="19"/>
       <c r="C6" s="1">
         <v>30.0</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="F6" s="1">
         <v>5.0</v>
@@ -941,16 +962,16 @@
     </row>
     <row r="7">
       <c r="A7" s="1" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="B7" s="13" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="F7" s="1">
         <v>5.0</v>
@@ -958,16 +979,16 @@
     </row>
     <row r="8">
       <c r="A8" s="1" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="B8" s="13" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="C8" s="1">
         <v>30.0</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="F8" s="1">
         <v>5.0</v>
@@ -975,16 +996,16 @@
     </row>
     <row r="9">
       <c r="A9" s="1" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="B9" s="13" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="C9" s="1">
         <v>30.0</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="F9" s="1">
         <v>5.0</v>
@@ -992,27 +1013,27 @@
     </row>
     <row r="10">
       <c r="A10" s="1" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="B10" s="13" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="C10" s="1">
         <v>30.0</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="F11" s="1">
         <v>28.0</v>
@@ -1020,10 +1041,10 @@
     </row>
     <row r="12">
       <c r="A12" s="1" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="C12" s="13" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
class module by maheswari
</commit_message>
<xml_diff>
--- a/src/test/resources/LMSData.xlsx
+++ b/src/test/resources/LMSData.xlsx
@@ -880,7 +880,7 @@
         <v>42</v>
       </c>
       <c r="C2" s="15">
-        <v>24.0</v>
+        <v>27.0</v>
       </c>
       <c r="D2" s="16" t="s">
         <v>43</v>
@@ -920,7 +920,7 @@
         <v>42</v>
       </c>
       <c r="C4" s="19">
-        <v>25.0</v>
+        <v>28.0</v>
       </c>
       <c r="D4" s="10" t="s">
         <v>48</v>
@@ -940,7 +940,7 @@
         <v>42</v>
       </c>
       <c r="C5" s="19">
-        <v>26.0</v>
+        <v>29.0</v>
       </c>
       <c r="D5" s="10" t="s">
         <v>50</v>

</xml_diff>